<commit_message>
Updated graphs. Recreated allexpfiles22.csv file.
</commit_message>
<xml_diff>
--- a/summary_file_droppeCOVIDrevs_FY2022.xlsx
+++ b/summary_file_droppeCOVIDrevs_FY2022.xlsx
@@ -21937,7 +21937,7 @@
         <v>59</v>
       </c>
       <c r="D696" t="n">
-        <v>1897.14146819</v>
+        <v>1676.31878603</v>
       </c>
       <c r="E696" t="s">
         <v>60</v>
@@ -22447,7 +22447,7 @@
         <v>59</v>
       </c>
       <c r="D726" t="n">
-        <v>1410.09469536</v>
+        <v>1391.12864775</v>
       </c>
       <c r="E726" t="s">
         <v>60</v>
@@ -22566,7 +22566,7 @@
         <v>73</v>
       </c>
       <c r="D733" t="n">
-        <v>2205.55107932</v>
+        <v>1834.46138382</v>
       </c>
       <c r="E733" t="s">
         <v>74</v>
@@ -23034,44 +23034,44 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="B11" t="n">
-        <v>2.2</v>
+        <v>2.1</v>
       </c>
       <c r="C11" t="n">
-        <v>31.4</v>
+        <v>7.06</v>
       </c>
       <c r="D11" t="n">
-        <v>7.15</v>
+        <v>7.54</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>80</v>
+        <v>108</v>
       </c>
       <c r="B12" t="n">
-        <v>2.1</v>
+        <v>2</v>
       </c>
       <c r="C12" t="n">
-        <v>7.06</v>
+        <v>-0.83</v>
       </c>
       <c r="D12" t="n">
-        <v>7.54</v>
+        <v>6.11</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>108</v>
+        <v>74</v>
       </c>
       <c r="B13" t="n">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.83</v>
+        <v>9.29</v>
       </c>
       <c r="D13" t="n">
-        <v>6.11</v>
+        <v>6.33</v>
       </c>
     </row>
     <row r="14">
@@ -23110,10 +23110,10 @@
         <v>1.4</v>
       </c>
       <c r="C16" t="n">
-        <v>-25.67</v>
+        <v>-17.01</v>
       </c>
       <c r="D16" t="n">
-        <v>4.73</v>
+        <v>4.67</v>
       </c>
     </row>
     <row r="17">
@@ -24385,22 +24385,22 @@
         <v>60</v>
       </c>
       <c r="B8" t="n">
-        <v>-25.67</v>
+        <v>-17.01</v>
       </c>
       <c r="C8" t="n">
-        <v>50.78</v>
+        <v>49.77</v>
       </c>
       <c r="D8" t="n">
-        <v>34.76</v>
+        <v>34.15</v>
       </c>
       <c r="E8" t="n">
-        <v>16.78</v>
+        <v>16.46</v>
       </c>
       <c r="F8" t="n">
-        <v>3.22</v>
+        <v>3.08</v>
       </c>
       <c r="G8" t="n">
-        <v>4.73</v>
+        <v>4.67</v>
       </c>
     </row>
     <row r="9">
@@ -24822,22 +24822,22 @@
         <v>74</v>
       </c>
       <c r="B27" t="n">
-        <v>31.4</v>
+        <v>9.29</v>
       </c>
       <c r="C27" t="n">
-        <v>39.94</v>
+        <v>27.63</v>
       </c>
       <c r="D27" t="n">
-        <v>54.41</v>
+        <v>45.21</v>
       </c>
       <c r="E27" t="n">
-        <v>35.09</v>
+        <v>30.21</v>
       </c>
       <c r="F27" t="n">
-        <v>15.96</v>
+        <v>13.84</v>
       </c>
       <c r="G27" t="n">
-        <v>7.15</v>
+        <v>6.33</v>
       </c>
     </row>
     <row r="28">
@@ -24962,170 +24962,170 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1998</v>
+        <v>2022</v>
       </c>
       <c r="B2" t="n">
-        <v>31218.4556557</v>
+        <v>99785.57583777</v>
       </c>
       <c r="C2" t="n">
-        <v>31264.6818251</v>
+        <v>104536.89862629</v>
       </c>
       <c r="D2" t="n">
-        <v>46</v>
+        <v>4751</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1999</v>
+        <v>2021</v>
       </c>
       <c r="B3" t="n">
-        <v>33804.96576153</v>
+        <v>92807.10818869</v>
       </c>
       <c r="C3" t="n">
-        <v>33030.24759485</v>
+        <v>91577.64567625</v>
       </c>
       <c r="D3" t="n">
-        <v>-775</v>
+        <v>-1229</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2000</v>
+        <v>2020</v>
       </c>
       <c r="B4" t="n">
-        <v>37283.0484234</v>
+        <v>81574.30708322</v>
       </c>
       <c r="C4" t="n">
-        <v>35846.01278232</v>
+        <v>74622.7453303</v>
       </c>
       <c r="D4" t="n">
-        <v>-1437</v>
+        <v>-6952</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>2001</v>
+        <v>2019</v>
       </c>
       <c r="B5" t="n">
-        <v>40300.24229108</v>
+        <v>74383.59556887</v>
       </c>
       <c r="C5" t="n">
-        <v>37147.74155936</v>
+        <v>72152.86792715</v>
       </c>
       <c r="D5" t="n">
-        <v>-3153</v>
+        <v>-2231</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>2002</v>
+        <v>2018</v>
       </c>
       <c r="B6" t="n">
-        <v>42014.32484476</v>
+        <v>74942.56778491</v>
       </c>
       <c r="C6" t="n">
-        <v>36825.92689326</v>
+        <v>70256.5668322</v>
       </c>
       <c r="D6" t="n">
-        <v>-5188</v>
+        <v>-4686</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>2003</v>
+        <v>2017</v>
       </c>
       <c r="B7" t="n">
-        <v>42567.13604378</v>
+        <v>71704.78677854</v>
       </c>
       <c r="C7" t="n">
-        <v>36805.69976915</v>
+        <v>60945.18463144</v>
       </c>
       <c r="D7" t="n">
-        <v>-5761</v>
+        <v>-10760</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>2004</v>
+        <v>2016</v>
       </c>
       <c r="B8" t="n">
-        <v>52980.20713006</v>
+        <v>63909.28178688</v>
       </c>
       <c r="C8" t="n">
-        <v>40856.23669512</v>
+        <v>61806.01279253</v>
       </c>
       <c r="D8" t="n">
-        <v>-12124</v>
+        <v>-2103</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>2005</v>
+        <v>2015</v>
       </c>
       <c r="B9" t="n">
-        <v>45331.21505246</v>
+        <v>69920.57755159</v>
       </c>
       <c r="C9" t="n">
-        <v>42865.85989889</v>
+        <v>63882.73647204</v>
       </c>
       <c r="D9" t="n">
-        <v>-2465</v>
+        <v>-6038</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>2006</v>
+        <v>2014</v>
       </c>
       <c r="B10" t="n">
-        <v>48028.45089847</v>
+        <v>66941.54371749</v>
       </c>
       <c r="C10" t="n">
-        <v>44700.58108122</v>
+        <v>62519.59401338</v>
       </c>
       <c r="D10" t="n">
-        <v>-3328</v>
+        <v>-4422</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>2007</v>
+        <v>2013</v>
       </c>
       <c r="B11" t="n">
-        <v>51098.59908858</v>
+        <v>63261.01592636</v>
       </c>
       <c r="C11" t="n">
-        <v>48033.24657002</v>
+        <v>60502.20379116</v>
       </c>
       <c r="D11" t="n">
-        <v>-3065</v>
+        <v>-2759</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>2008</v>
+        <v>2012</v>
       </c>
       <c r="B12" t="n">
-        <v>54138.63848686</v>
+        <v>59831.151018</v>
       </c>
       <c r="C12" t="n">
-        <v>50213.47771324</v>
+        <v>55452.47810214</v>
       </c>
       <c r="D12" t="n">
-        <v>-3925</v>
+        <v>-4379</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>2009</v>
+        <v>2011</v>
       </c>
       <c r="B13" t="n">
-        <v>56721.04766907</v>
+        <v>60403.66316511</v>
       </c>
       <c r="C13" t="n">
-        <v>49858.93285555</v>
+        <v>51719.80617799</v>
       </c>
       <c r="D13" t="n">
-        <v>-6862</v>
+        <v>-8684</v>
       </c>
     </row>
     <row r="14">
@@ -25136,178 +25136,178 @@
         <v>59247.71610651</v>
       </c>
       <c r="C14" t="n">
-        <v>49838.70244961</v>
+        <v>46059.51698249</v>
       </c>
       <c r="D14" t="n">
-        <v>-9409</v>
+        <v>-13188</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>2011</v>
+        <v>2009</v>
       </c>
       <c r="B15" t="n">
-        <v>60403.66316511</v>
+        <v>56721.04766907</v>
       </c>
       <c r="C15" t="n">
-        <v>54731.97018504</v>
+        <v>47822.53037459</v>
       </c>
       <c r="D15" t="n">
-        <v>-5672</v>
+        <v>-8899</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>2012</v>
+        <v>2008</v>
       </c>
       <c r="B16" t="n">
-        <v>59831.151018</v>
+        <v>54138.63848686</v>
       </c>
       <c r="C16" t="n">
-        <v>56248.09850297</v>
+        <v>50213.47771324</v>
       </c>
       <c r="D16" t="n">
-        <v>-3583</v>
+        <v>-3925</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>2013</v>
+        <v>2007</v>
       </c>
       <c r="B17" t="n">
-        <v>63261.01592636</v>
+        <v>51098.59908858</v>
       </c>
       <c r="C17" t="n">
-        <v>60804.21955684</v>
+        <v>48033.24657002</v>
       </c>
       <c r="D17" t="n">
-        <v>-2457</v>
+        <v>-3065</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>2014</v>
+        <v>2006</v>
       </c>
       <c r="B18" t="n">
-        <v>66941.54371749</v>
+        <v>48028.45089847</v>
       </c>
       <c r="C18" t="n">
-        <v>62772.23529438</v>
+        <v>44700.58108122</v>
       </c>
       <c r="D18" t="n">
-        <v>-4169</v>
+        <v>-3328</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>2015</v>
+        <v>2005</v>
       </c>
       <c r="B19" t="n">
-        <v>69920.57755159</v>
+        <v>45331.21505246</v>
       </c>
       <c r="C19" t="n">
-        <v>64113.55535379</v>
+        <v>42865.85989889</v>
       </c>
       <c r="D19" t="n">
-        <v>-5807</v>
+        <v>-2465</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>2016</v>
+        <v>2004</v>
       </c>
       <c r="B20" t="n">
-        <v>63909.28178688</v>
+        <v>52980.20713006</v>
       </c>
       <c r="C20" t="n">
-        <v>61985.5590092</v>
+        <v>40856.23669512</v>
       </c>
       <c r="D20" t="n">
-        <v>-1924</v>
+        <v>-12124</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>2017</v>
+        <v>2003</v>
       </c>
       <c r="B21" t="n">
-        <v>71704.78677854</v>
+        <v>42567.13604378</v>
       </c>
       <c r="C21" t="n">
-        <v>61349.20521982</v>
+        <v>36805.69976915</v>
       </c>
       <c r="D21" t="n">
-        <v>-10356</v>
+        <v>-5761</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>2018</v>
+        <v>2002</v>
       </c>
       <c r="B22" t="n">
-        <v>74942.56778491</v>
+        <v>42014.32484476</v>
       </c>
       <c r="C22" t="n">
-        <v>70465.15077644</v>
+        <v>36825.92689326</v>
       </c>
       <c r="D22" t="n">
-        <v>-4477</v>
+        <v>-5188</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>2019</v>
+        <v>2001</v>
       </c>
       <c r="B23" t="n">
-        <v>74383.59556887</v>
+        <v>40300.24229108</v>
       </c>
       <c r="C23" t="n">
-        <v>72152.86792715</v>
+        <v>37147.74155936</v>
       </c>
       <c r="D23" t="n">
-        <v>-2231</v>
+        <v>-3153</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>2020</v>
+        <v>2000</v>
       </c>
       <c r="B24" t="n">
-        <v>81574.30708322</v>
+        <v>37283.0484234</v>
       </c>
       <c r="C24" t="n">
-        <v>78141.690696</v>
+        <v>35846.01278232</v>
       </c>
       <c r="D24" t="n">
-        <v>-3433</v>
+        <v>-1437</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>2021</v>
+        <v>1999</v>
       </c>
       <c r="B25" t="n">
-        <v>93027.93087085</v>
+        <v>33804.96576153</v>
       </c>
       <c r="C25" t="n">
-        <v>91806.06006519</v>
+        <v>33030.24759485</v>
       </c>
       <c r="D25" t="n">
-        <v>-1222</v>
+        <v>-775</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>2022</v>
+        <v>1998</v>
       </c>
       <c r="B26" t="n">
-        <v>100175.63158088</v>
+        <v>31218.4556557</v>
       </c>
       <c r="C26" t="n">
-        <v>113392.64805172</v>
+        <v>31264.6818251</v>
       </c>
       <c r="D26" t="n">
-        <v>13217</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>